<commit_message>
work from the plane
</commit_message>
<xml_diff>
--- a/svc-prosody.xlsx
+++ b/svc-prosody.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npeck\Documents\R\svc-prosody\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D19664B-21CA-476B-9483-B5B58EA005A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9AC694-D7C9-4E89-8DBB-3990E0437974}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8856" xr2:uid="{084F7C11-1A98-4603-980E-4D67AF5CB169}"/>
   </bookViews>
@@ -1898,10 +1898,10 @@
   <dimension ref="A1:G202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E77" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F171" sqref="F171"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1936,14 +1936,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>347</v>
+      <c r="A2" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="B2" t="s">
-        <v>348</v>
+        <v>272</v>
       </c>
       <c r="C2" t="s">
-        <v>349</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>270</v>
@@ -1951,8 +1951,8 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>0</v>
+      <c r="F2" t="s">
+        <v>457</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1960,33 +1960,33 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>376</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>485</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
+        <v>464</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
+      <c r="F3" t="s">
+        <v>457</v>
+      </c>
+      <c r="G3" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>409</v>
+        <v>487</v>
       </c>
       <c r="B4" t="s">
-        <v>410</v>
+        <v>379</v>
       </c>
       <c r="C4" t="s">
         <v>207</v>
@@ -1997,45 +1997,45 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="F4" t="s">
+        <v>457</v>
       </c>
       <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>372</v>
+        <v>287</v>
       </c>
       <c r="B5" t="s">
-        <v>373</v>
+        <v>288</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>287</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>0</v>
+      <c r="F5" t="s">
+        <v>457</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>370</v>
+      <c r="A6" t="s">
+        <v>347</v>
       </c>
       <c r="B6" t="s">
-        <v>371</v>
+        <v>348</v>
       </c>
       <c r="C6" t="s">
-        <v>207</v>
+        <v>349</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>270</v>
@@ -2050,18 +2050,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>188</v>
+        <v>83</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2069,28 +2069,28 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>481</v>
+        <v>167</v>
       </c>
       <c r="B8" t="s">
-        <v>482</v>
+        <v>168</v>
       </c>
       <c r="C8" t="s">
-        <v>227</v>
+        <v>169</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>0</v>
+      <c r="F8" t="s">
+        <v>457</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -2098,177 +2098,177 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>368</v>
+        <v>273</v>
       </c>
       <c r="B9" t="s">
-        <v>369</v>
+        <v>274</v>
       </c>
       <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>457</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>262</v>
+      </c>
+      <c r="B10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C10" t="s">
+        <v>255</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>457</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>362</v>
+      </c>
+      <c r="B12" t="s">
+        <v>363</v>
+      </c>
+      <c r="C12" t="s">
         <v>207</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>316</v>
-      </c>
-      <c r="B11" t="s">
-        <v>317</v>
-      </c>
-      <c r="C11" t="s">
-        <v>318</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12" t="s">
-        <v>228</v>
-      </c>
-      <c r="C12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>230</v>
-      </c>
-      <c r="B13" t="s">
-        <v>231</v>
-      </c>
-      <c r="C13" t="s">
-        <v>227</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13">
-        <v>0</v>
+      <c r="F13" t="s">
+        <v>457</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>386</v>
+      <c r="A14" s="2" t="s">
+        <v>471</v>
       </c>
       <c r="B14" t="s">
-        <v>387</v>
+        <v>472</v>
       </c>
       <c r="C14" t="s">
-        <v>207</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>270</v>
+        <v>13</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
+      <c r="F14" t="s">
+        <v>457</v>
+      </c>
+      <c r="G14" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>384</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>385</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>207</v>
+        <v>463</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15">
-        <v>0</v>
+      <c r="F15" t="s">
+        <v>457</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>430</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>431</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>207</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>270</v>
+        <v>18</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -2276,65 +2276,65 @@
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>217</v>
+      <c r="G16" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>479</v>
       </c>
       <c r="B17" t="s">
-        <v>218</v>
+        <v>480</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17">
-        <v>0</v>
+      <c r="F17" t="s">
+        <v>457</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>388</v>
+        <v>140</v>
       </c>
       <c r="B18" t="s">
-        <v>389</v>
+        <v>142</v>
       </c>
       <c r="C18" t="s">
-        <v>207</v>
+        <v>141</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18">
-        <v>0</v>
+      <c r="F18" t="s">
+        <v>457</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>467</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>468</v>
       </c>
       <c r="C19" t="s">
-        <v>464</v>
+        <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>14</v>
@@ -2342,68 +2342,68 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>457</v>
+      </c>
+      <c r="G19" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>223</v>
+        <v>306</v>
       </c>
       <c r="B20" t="s">
-        <v>224</v>
+        <v>307</v>
       </c>
       <c r="C20" t="s">
-        <v>225</v>
+        <v>308</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21">
-        <v>0</v>
+      <c r="F21" t="s">
+        <v>457</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>352</v>
+      <c r="A22" t="s">
+        <v>376</v>
       </c>
       <c r="B22" t="s">
-        <v>353</v>
+        <v>485</v>
       </c>
       <c r="C22" t="s">
-        <v>354</v>
+        <v>207</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>270</v>
@@ -2420,39 +2420,39 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>392</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>393</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>409</v>
+      </c>
+      <c r="B24" t="s">
+        <v>410</v>
+      </c>
+      <c r="C24" t="s">
         <v>207</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>264</v>
-      </c>
-      <c r="B24" t="s">
-        <v>265</v>
-      </c>
-      <c r="C24" t="s">
-        <v>266</v>
-      </c>
       <c r="D24" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -2464,15 +2464,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>236</v>
+        <v>372</v>
       </c>
       <c r="B25" t="s">
-        <v>237</v>
+        <v>373</v>
       </c>
       <c r="C25" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>12</v>
@@ -2489,13 +2489,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>309</v>
+        <v>370</v>
       </c>
       <c r="B26" t="s">
-        <v>310</v>
+        <v>371</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>207</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>270</v>
@@ -2511,17 +2511,17 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>292</v>
+      <c r="A27" t="s">
+        <v>189</v>
       </c>
       <c r="B27" t="s">
-        <v>293</v>
+        <v>190</v>
       </c>
       <c r="C27" t="s">
-        <v>291</v>
+        <v>188</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>270</v>
+        <v>12</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -2533,41 +2533,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>491</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>492</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
+      <c r="F28" t="s">
+        <v>457</v>
+      </c>
+      <c r="G28" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>278</v>
+        <v>481</v>
       </c>
       <c r="B29" t="s">
-        <v>280</v>
+        <v>482</v>
       </c>
       <c r="C29" t="s">
-        <v>279</v>
+        <v>227</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>270</v>
+        <v>12</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -2579,18 +2579,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>213</v>
+        <v>368</v>
       </c>
       <c r="B30" t="s">
-        <v>214</v>
+        <v>369</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>207</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -2630,15 +2630,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>215</v>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>191</v>
       </c>
       <c r="B33" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>12</v>
@@ -2646,192 +2646,192 @@
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="F33">
-        <v>0</v>
+      <c r="F33" t="s">
+        <v>457</v>
       </c>
       <c r="G33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>456</v>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>475</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>476</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>465</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
+      <c r="F34" t="s">
+        <v>457</v>
+      </c>
+      <c r="G34" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>417</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>418</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>457</v>
+      </c>
+      <c r="G35" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>380</v>
+      </c>
+      <c r="B36" t="s">
+        <v>381</v>
+      </c>
+      <c r="C36" t="s">
         <v>207</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C36" t="s">
-        <v>19</v>
-      </c>
       <c r="D36" s="1" t="s">
-        <v>18</v>
+        <v>270</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>324</v>
+      <c r="A37" t="s">
+        <v>164</v>
       </c>
       <c r="B37" t="s">
-        <v>325</v>
+        <v>165</v>
       </c>
       <c r="C37" t="s">
-        <v>326</v>
+        <v>166</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>457</v>
+      </c>
+      <c r="G37" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="B38" t="s">
-        <v>180</v>
+        <v>489</v>
       </c>
       <c r="C38" t="s">
-        <v>181</v>
+        <v>227</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>457</v>
+      </c>
+      <c r="G38" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B39" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>267</v>
-      </c>
-      <c r="B39" t="s">
-        <v>268</v>
-      </c>
-      <c r="C39" t="s">
-        <v>269</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="F39">
-        <v>0</v>
+      <c r="F39" t="s">
+        <v>457</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>423</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>424</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>382</v>
+      </c>
+      <c r="B41" t="s">
+        <v>383</v>
+      </c>
+      <c r="C41" t="s">
         <v>207</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" t="s">
-        <v>147</v>
-      </c>
-      <c r="C41" t="s">
-        <v>148</v>
-      </c>
       <c r="D41" s="1" t="s">
-        <v>14</v>
+        <v>270</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41">
-        <v>0</v>
+      <c r="F41" t="s">
+        <v>457</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2839,13 +2839,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>306</v>
+        <v>488</v>
       </c>
       <c r="B42" t="s">
-        <v>307</v>
+        <v>345</v>
       </c>
       <c r="C42" t="s">
-        <v>308</v>
+        <v>346</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>270</v>
@@ -2854,10 +2854,10 @@
         <v>1</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -2876,13 +2876,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>380</v>
+        <v>316</v>
       </c>
       <c r="B44" t="s">
-        <v>381</v>
+        <v>317</v>
       </c>
       <c r="C44" t="s">
-        <v>207</v>
+        <v>318</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>270</v>
@@ -2891,7 +2891,7 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -2899,22 +2899,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>358</v>
+        <v>226</v>
       </c>
       <c r="B45" t="s">
-        <v>359</v>
+        <v>228</v>
       </c>
       <c r="C45" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>270</v>
+        <v>12</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -2922,68 +2922,68 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>429</v>
+        <v>289</v>
       </c>
       <c r="B46" t="s">
-        <v>490</v>
+        <v>290</v>
       </c>
       <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>230</v>
+      </c>
+      <c r="B47" t="s">
+        <v>231</v>
+      </c>
+      <c r="C47" t="s">
+        <v>227</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>386</v>
+      </c>
+      <c r="B48" t="s">
+        <v>387</v>
+      </c>
+      <c r="C48" t="s">
         <v>207</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B47" t="s">
-        <v>272</v>
-      </c>
-      <c r="C47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>457</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>167</v>
-      </c>
-      <c r="B48" t="s">
-        <v>168</v>
-      </c>
-      <c r="C48" t="s">
-        <v>169</v>
-      </c>
       <c r="D48" s="1" t="s">
-        <v>14</v>
+        <v>270</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="F48" t="s">
-        <v>457</v>
+      <c r="F48">
+        <v>0</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2991,13 +2991,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>273</v>
+        <v>384</v>
       </c>
       <c r="B49" t="s">
-        <v>274</v>
+        <v>385</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>207</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>270</v>
@@ -3005,48 +3005,48 @@
       <c r="E49">
         <v>1</v>
       </c>
-      <c r="F49" t="s">
-        <v>457</v>
+      <c r="F49">
+        <v>0</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>262</v>
+        <v>430</v>
       </c>
       <c r="B50" t="s">
-        <v>263</v>
+        <v>431</v>
       </c>
       <c r="C50" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
-      <c r="F50" t="s">
-        <v>457</v>
+      <c r="F50">
+        <v>0</v>
       </c>
       <c r="G50">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>62</v>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -3054,8 +3054,8 @@
       <c r="F51" t="s">
         <v>457</v>
       </c>
-      <c r="G51">
-        <v>0</v>
+      <c r="G51" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -3072,64 +3072,64 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>217</v>
       </c>
       <c r="B53" t="s">
-        <v>142</v>
+        <v>218</v>
       </c>
       <c r="C53" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="D53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B54" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" t="s">
+        <v>463</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E53">
-        <v>1</v>
-      </c>
-      <c r="F53" t="s">
-        <v>457</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>191</v>
-      </c>
-      <c r="B54" t="s">
-        <v>192</v>
-      </c>
-      <c r="C54" t="s">
-        <v>188</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54" t="s">
-        <v>457</v>
+      <c r="F54">
+        <v>0</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>382</v>
+        <v>99</v>
       </c>
       <c r="B55" t="s">
-        <v>383</v>
+        <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>207</v>
+        <v>98</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>270</v>
+        <v>13</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -3137,8 +3137,8 @@
       <c r="F55" t="s">
         <v>457</v>
       </c>
-      <c r="G55">
-        <v>0</v>
+      <c r="G55" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -3171,13 +3171,13 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>300</v>
+        <v>388</v>
       </c>
       <c r="B58" t="s">
-        <v>301</v>
+        <v>389</v>
       </c>
       <c r="C58" t="s">
-        <v>302</v>
+        <v>207</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>270</v>
@@ -3185,31 +3185,31 @@
       <c r="E58">
         <v>1</v>
       </c>
-      <c r="F58" t="s">
-        <v>457</v>
+      <c r="F58">
+        <v>0</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>322</v>
+      <c r="A59" t="s">
+        <v>110</v>
       </c>
       <c r="B59" t="s">
-        <v>323</v>
+        <v>111</v>
       </c>
       <c r="C59" t="s">
-        <v>321</v>
+        <v>464</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
-      <c r="F59" t="s">
-        <v>457</v>
+      <c r="F59">
+        <v>0</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -3229,42 +3229,42 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>234</v>
+        <v>7</v>
       </c>
       <c r="B61" t="s">
-        <v>235</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>457</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>245</v>
+      </c>
+      <c r="B62" t="s">
+        <v>246</v>
+      </c>
+      <c r="C62" t="s">
         <v>227</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="F61" t="s">
-        <v>457</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>80</v>
-      </c>
-      <c r="B62" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E62">
         <v>1</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>457</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -3289,18 +3289,18 @@
         <v>270</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
-        <v>240</v>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>340</v>
       </c>
       <c r="B64" t="s">
-        <v>241</v>
+        <v>341</v>
       </c>
       <c r="C64" t="s">
-        <v>227</v>
+        <v>342</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -3309,21 +3309,21 @@
         <v>457</v>
       </c>
       <c r="G64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>256</v>
+        <v>300</v>
       </c>
       <c r="B65" t="s">
-        <v>257</v>
+        <v>301</v>
       </c>
       <c r="C65" t="s">
-        <v>255</v>
+        <v>302</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -3336,17 +3336,17 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>281</v>
+      <c r="A66" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>282</v>
+        <v>31</v>
       </c>
       <c r="C66" t="s">
-        <v>283</v>
+        <v>32</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>270</v>
+        <v>13</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -3355,21 +3355,21 @@
         <v>457</v>
       </c>
       <c r="G66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>242</v>
+        <v>37</v>
       </c>
       <c r="B67" t="s">
-        <v>243</v>
+        <v>38</v>
       </c>
       <c r="C67" t="s">
-        <v>227</v>
+        <v>39</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -3378,18 +3378,18 @@
         <v>457</v>
       </c>
       <c r="G67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B68" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C68" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>12</v>
@@ -3397,25 +3397,25 @@
       <c r="E68">
         <v>1</v>
       </c>
-      <c r="F68" t="s">
-        <v>457</v>
+      <c r="F68">
+        <v>0</v>
       </c>
       <c r="G68">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>149</v>
+        <v>193</v>
       </c>
       <c r="B69" t="s">
-        <v>150</v>
+        <v>194</v>
       </c>
       <c r="C69" t="s">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -3423,8 +3423,8 @@
       <c r="F69" t="s">
         <v>457</v>
       </c>
-      <c r="G69">
-        <v>0</v>
+      <c r="G69" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -3441,41 +3441,41 @@
         <v>270</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>201</v>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B71" t="s">
-        <v>202</v>
+        <v>52</v>
       </c>
       <c r="C71" t="s">
-        <v>188</v>
+        <v>20</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E71">
         <v>1</v>
       </c>
-      <c r="F71" t="s">
-        <v>457</v>
+      <c r="F71">
+        <v>0</v>
       </c>
       <c r="G71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>203</v>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="B72" t="s">
-        <v>204</v>
+        <v>323</v>
       </c>
       <c r="C72" t="s">
-        <v>188</v>
+        <v>321</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -3487,65 +3487,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
-        <v>154</v>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>284</v>
       </c>
       <c r="B73" t="s">
-        <v>155</v>
-      </c>
-      <c r="C73" t="s">
-        <v>9</v>
+        <v>285</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>286</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>14</v>
+        <v>270</v>
       </c>
       <c r="E73">
         <v>1</v>
       </c>
-      <c r="F73" t="s">
-        <v>457</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>28</v>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>352</v>
       </c>
       <c r="B74" t="s">
-        <v>29</v>
+        <v>353</v>
       </c>
       <c r="C74" t="s">
-        <v>27</v>
+        <v>354</v>
       </c>
       <c r="D74" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E74">
-        <v>1</v>
-      </c>
-      <c r="F74" t="s">
-        <v>457</v>
-      </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>258</v>
-      </c>
-      <c r="B75" t="s">
-        <v>259</v>
-      </c>
-      <c r="C75" t="s">
-        <v>255</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E75">
         <v>1</v>
       </c>
@@ -3553,18 +3553,18 @@
         <v>457</v>
       </c>
       <c r="G75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="B76" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="C76" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>14</v>
@@ -3576,18 +3576,18 @@
         <v>457</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>364</v>
+      <c r="A77" s="2" t="s">
+        <v>454</v>
       </c>
       <c r="B77" t="s">
-        <v>365</v>
+        <v>455</v>
       </c>
       <c r="C77" t="s">
-        <v>207</v>
+        <v>329</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>270</v>
@@ -3595,11 +3595,11 @@
       <c r="E77">
         <v>1</v>
       </c>
-      <c r="F77" t="s">
-        <v>457</v>
+      <c r="F77">
+        <v>0</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -3630,18 +3630,18 @@
         <v>270</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>170</v>
+        <v>234</v>
       </c>
       <c r="B80" t="s">
-        <v>171</v>
+        <v>235</v>
       </c>
       <c r="C80" t="s">
-        <v>172</v>
+        <v>227</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -3655,16 +3655,16 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>411</v>
+        <v>46</v>
       </c>
       <c r="B81" t="s">
-        <v>412</v>
+        <v>47</v>
       </c>
       <c r="C81" t="s">
-        <v>207</v>
+        <v>21</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>270</v>
+        <v>18</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -3672,19 +3672,19 @@
       <c r="F81" t="s">
         <v>457</v>
       </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G81" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C82" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>71</v>
@@ -3701,13 +3701,13 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>488</v>
+        <v>392</v>
       </c>
       <c r="B83" t="s">
-        <v>345</v>
+        <v>393</v>
       </c>
       <c r="C83" t="s">
-        <v>346</v>
+        <v>207</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>270</v>
@@ -3719,21 +3719,21 @@
         <v>0</v>
       </c>
       <c r="G83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>120</v>
+        <v>264</v>
       </c>
       <c r="B84" t="s">
-        <v>121</v>
+        <v>265</v>
       </c>
       <c r="C84" t="s">
-        <v>463</v>
+        <v>266</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -3742,21 +3742,21 @@
         <v>0</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
-        <v>454</v>
+      <c r="A85" t="s">
+        <v>236</v>
       </c>
       <c r="B85" t="s">
-        <v>455</v>
+        <v>237</v>
       </c>
       <c r="C85" t="s">
-        <v>329</v>
+        <v>227</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>270</v>
+        <v>12</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -3765,41 +3765,41 @@
         <v>0</v>
       </c>
       <c r="G85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>311</v>
+      <c r="A86" t="s">
+        <v>232</v>
       </c>
       <c r="B86" t="s">
-        <v>312</v>
+        <v>233</v>
       </c>
       <c r="C86" t="s">
-        <v>9</v>
+        <v>227</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>270</v>
+        <v>12</v>
       </c>
       <c r="E86">
         <v>1</v>
       </c>
-      <c r="F86">
-        <v>0</v>
-      </c>
-      <c r="G86">
-        <v>1</v>
+      <c r="F86" t="s">
+        <v>457</v>
+      </c>
+      <c r="G86" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
       <c r="B87" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="C87" t="s">
-        <v>9</v>
+        <v>299</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>270</v>
@@ -3807,11 +3807,11 @@
       <c r="E87">
         <v>1</v>
       </c>
-      <c r="F87">
-        <v>0</v>
-      </c>
-      <c r="G87">
-        <v>1</v>
+      <c r="F87" t="s">
+        <v>457</v>
+      </c>
+      <c r="G87" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -3828,15 +3828,15 @@
         <v>270</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>114</v>
+        <v>176</v>
       </c>
       <c r="B89" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
       <c r="C89" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>14</v>
@@ -3844,11 +3844,11 @@
       <c r="E89">
         <v>1</v>
       </c>
-      <c r="F89">
-        <v>0</v>
-      </c>
-      <c r="G89">
-        <v>1</v>
+      <c r="F89" t="s">
+        <v>457</v>
+      </c>
+      <c r="G89" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -3866,63 +3866,63 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
-        <v>343</v>
+      <c r="A91" t="s">
+        <v>211</v>
       </c>
       <c r="B91" t="s">
-        <v>344</v>
+        <v>212</v>
       </c>
       <c r="C91" t="s">
+        <v>17</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91">
+        <v>1</v>
+      </c>
+      <c r="F91" t="s">
+        <v>457</v>
+      </c>
+      <c r="G91" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B92" t="s">
+        <v>310</v>
+      </c>
+      <c r="C92" t="s">
         <v>9</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E91">
-        <v>1</v>
-      </c>
-      <c r="F91">
-        <v>0</v>
-      </c>
-      <c r="G91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>487</v>
-      </c>
-      <c r="B92" t="s">
-        <v>379</v>
-      </c>
-      <c r="C92" t="s">
-        <v>207</v>
-      </c>
       <c r="D92" s="1" t="s">
         <v>270</v>
       </c>
       <c r="E92">
         <v>1</v>
       </c>
-      <c r="F92" t="s">
-        <v>457</v>
+      <c r="F92">
+        <v>0</v>
       </c>
       <c r="G92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>287</v>
+        <v>260</v>
       </c>
       <c r="B93" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
       <c r="C93" t="s">
-        <v>287</v>
+        <v>255</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>270</v>
+        <v>12</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -3930,8 +3930,8 @@
       <c r="F93" t="s">
         <v>457</v>
       </c>
-      <c r="G93">
-        <v>1</v>
+      <c r="G93" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -3948,18 +3948,18 @@
         <v>270</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>116</v>
+        <v>240</v>
       </c>
       <c r="B95" t="s">
-        <v>117</v>
+        <v>241</v>
       </c>
       <c r="C95" t="s">
-        <v>463</v>
+        <v>227</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -3968,21 +3968,21 @@
         <v>457</v>
       </c>
       <c r="G95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
-        <v>479</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>256</v>
       </c>
       <c r="B96" t="s">
-        <v>480</v>
+        <v>257</v>
       </c>
       <c r="C96" t="s">
-        <v>185</v>
+        <v>255</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -3991,7 +3991,7 @@
         <v>457</v>
       </c>
       <c r="G96">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -4008,24 +4008,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>92</v>
+        <v>311</v>
       </c>
       <c r="B98" t="s">
-        <v>93</v>
+        <v>312</v>
       </c>
       <c r="C98" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>71</v>
+        <v>270</v>
       </c>
       <c r="E98">
         <v>1</v>
       </c>
-      <c r="F98" t="s">
-        <v>457</v>
+      <c r="F98">
+        <v>0</v>
       </c>
       <c r="G98">
         <v>1</v>
@@ -4059,18 +4059,18 @@
         <v>270</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
-        <v>159</v>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>96</v>
       </c>
       <c r="B101" t="s">
-        <v>160</v>
+        <v>97</v>
       </c>
       <c r="C101" t="s">
-        <v>158</v>
+        <v>95</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -4078,22 +4078,22 @@
       <c r="F101" t="s">
         <v>457</v>
       </c>
-      <c r="G101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G101" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>7</v>
+        <v>401</v>
       </c>
       <c r="B102" t="s">
-        <v>8</v>
+        <v>402</v>
       </c>
       <c r="C102" t="s">
-        <v>9</v>
+        <v>207</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>13</v>
+        <v>270</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -4101,8 +4101,8 @@
       <c r="F102" t="s">
         <v>457</v>
       </c>
-      <c r="G102">
-        <v>1</v>
+      <c r="G102" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -4119,65 +4119,65 @@
         <v>270</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>245</v>
+        <v>281</v>
       </c>
       <c r="B104" t="s">
-        <v>246</v>
+        <v>282</v>
       </c>
       <c r="C104" t="s">
+        <v>283</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104" t="s">
+        <v>457</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>358</v>
+      </c>
+      <c r="B105" t="s">
+        <v>359</v>
+      </c>
+      <c r="C105" t="s">
+        <v>207</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>242</v>
+      </c>
+      <c r="B106" t="s">
+        <v>243</v>
+      </c>
+      <c r="C106" t="s">
         <v>227</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D106" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E104">
-        <v>1</v>
-      </c>
-      <c r="F104" t="s">
-        <v>457</v>
-      </c>
-      <c r="G104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="B105" t="s">
-        <v>341</v>
-      </c>
-      <c r="C105" t="s">
-        <v>342</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E105">
-        <v>1</v>
-      </c>
-      <c r="F105" t="s">
-        <v>457</v>
-      </c>
-      <c r="G105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B106" t="s">
-        <v>31</v>
-      </c>
-      <c r="C106" t="s">
-        <v>32</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E106">
         <v>1</v>
       </c>
@@ -4185,21 +4185,21 @@
         <v>457</v>
       </c>
       <c r="G106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>37</v>
+        <v>221</v>
       </c>
       <c r="B107" t="s">
-        <v>38</v>
+        <v>222</v>
       </c>
       <c r="C107" t="s">
-        <v>39</v>
+        <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -4208,21 +4208,21 @@
         <v>457</v>
       </c>
       <c r="G107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>44</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>56</v>
+      </c>
+      <c r="B108" t="s">
+        <v>57</v>
       </c>
       <c r="C108" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -4234,18 +4234,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>144</v>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B109" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
       <c r="C109" t="s">
-        <v>143</v>
+        <v>75</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -4253,28 +4253,28 @@
       <c r="F109" t="s">
         <v>457</v>
       </c>
-      <c r="G109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>56</v>
+      <c r="G109" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="B110" t="s">
-        <v>57</v>
+        <v>320</v>
       </c>
       <c r="C110" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>18</v>
+        <v>270</v>
       </c>
       <c r="E110">
         <v>1</v>
       </c>
-      <c r="F110" t="s">
-        <v>457</v>
+      <c r="F110">
+        <v>0</v>
       </c>
       <c r="G110">
         <v>1</v>
@@ -4294,18 +4294,18 @@
         <v>270</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
-        <v>477</v>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>275</v>
       </c>
       <c r="B112" t="s">
-        <v>478</v>
+        <v>277</v>
       </c>
       <c r="C112" t="s">
-        <v>6</v>
+        <v>276</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>14</v>
+        <v>270</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -4313,54 +4313,54 @@
       <c r="F112" t="s">
         <v>457</v>
       </c>
-      <c r="G112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>128</v>
+      <c r="G112" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="B113" t="s">
-        <v>129</v>
+        <v>295</v>
       </c>
       <c r="C113" t="s">
-        <v>466</v>
+        <v>296</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>14</v>
+        <v>270</v>
       </c>
       <c r="E113">
         <v>1</v>
       </c>
-      <c r="F113" t="s">
-        <v>457</v>
-      </c>
-      <c r="G113">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>469</v>
+        <v>292</v>
       </c>
       <c r="B114" t="s">
-        <v>470</v>
+        <v>293</v>
       </c>
       <c r="C114" t="s">
-        <v>143</v>
+        <v>291</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>14</v>
+        <v>270</v>
       </c>
       <c r="E114">
         <v>1</v>
       </c>
-      <c r="F114" t="s">
-        <v>457</v>
+      <c r="F114">
+        <v>0</v>
       </c>
       <c r="G114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -4377,50 +4377,50 @@
         <v>270</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>24</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>26</v>
+        <v>491</v>
+      </c>
+      <c r="B116" t="s">
+        <v>492</v>
       </c>
       <c r="C116" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E116">
         <v>1</v>
       </c>
-      <c r="F116" t="s">
-        <v>457</v>
+      <c r="F116">
+        <v>0</v>
       </c>
       <c r="G116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>130</v>
+        <v>278</v>
       </c>
       <c r="B117" t="s">
-        <v>131</v>
+        <v>280</v>
       </c>
       <c r="C117" t="s">
-        <v>465</v>
+        <v>279</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>14</v>
+        <v>270</v>
       </c>
       <c r="E117">
         <v>1</v>
       </c>
-      <c r="F117" t="s">
-        <v>457</v>
+      <c r="F117">
+        <v>0</v>
       </c>
       <c r="G117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -4437,18 +4437,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>15</v>
+        <v>199</v>
       </c>
       <c r="B119" t="s">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="C119" t="s">
-        <v>17</v>
+        <v>188</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E119">
         <v>1</v>
@@ -4456,19 +4456,19 @@
       <c r="F119" t="s">
         <v>457</v>
       </c>
-      <c r="G119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G119" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="B120" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
       <c r="C120" t="s">
-        <v>162</v>
+        <v>6</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>14</v>
@@ -4476,45 +4476,45 @@
       <c r="E120">
         <v>1</v>
       </c>
-      <c r="F120" t="s">
-        <v>457</v>
+      <c r="F120">
+        <v>0</v>
       </c>
       <c r="G120">
         <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>440</v>
+      <c r="A121" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B121" t="s">
-        <v>441</v>
+        <v>89</v>
       </c>
       <c r="C121" t="s">
-        <v>207</v>
+        <v>79</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>270</v>
+        <v>71</v>
       </c>
       <c r="E121">
         <v>1</v>
       </c>
-      <c r="F121" t="s">
-        <v>457</v>
-      </c>
-      <c r="G121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="G121" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>483</v>
+        <v>149</v>
       </c>
       <c r="B122" t="s">
-        <v>484</v>
+        <v>150</v>
       </c>
       <c r="C122" t="s">
-        <v>465</v>
+        <v>151</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>14</v>
@@ -4526,7 +4526,7 @@
         <v>457</v>
       </c>
       <c r="G122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -4543,50 +4543,50 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>82</v>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>477</v>
       </c>
       <c r="B124" t="s">
-        <v>90</v>
+        <v>478</v>
       </c>
       <c r="C124" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="E124">
         <v>1</v>
       </c>
-      <c r="F124">
-        <v>0</v>
-      </c>
-      <c r="G124" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="2" t="s">
-        <v>54</v>
+      <c r="F124" t="s">
+        <v>457</v>
+      </c>
+      <c r="G124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>128</v>
       </c>
       <c r="B125" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="C125" t="s">
-        <v>53</v>
+        <v>466</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E125">
         <v>1</v>
       </c>
-      <c r="F125">
-        <v>0</v>
-      </c>
-      <c r="G125" t="s">
-        <v>457</v>
+      <c r="F125" t="s">
+        <v>457</v>
+      </c>
+      <c r="G125">
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -4604,26 +4604,26 @@
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>362</v>
+      <c r="A127" s="2" t="s">
+        <v>469</v>
       </c>
       <c r="B127" t="s">
-        <v>363</v>
+        <v>470</v>
       </c>
       <c r="C127" t="s">
-        <v>207</v>
+        <v>143</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="E127">
         <v>1</v>
       </c>
-      <c r="F127">
-        <v>0</v>
-      </c>
-      <c r="G127" t="s">
-        <v>457</v>
+      <c r="F127" t="s">
+        <v>457</v>
+      </c>
+      <c r="G127">
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -4640,27 +4640,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>60</v>
-      </c>
-      <c r="B129" t="s">
-        <v>61</v>
+        <v>24</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C129" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E129">
         <v>1</v>
       </c>
-      <c r="F129">
-        <v>0</v>
-      </c>
-      <c r="G129" t="s">
-        <v>457</v>
+      <c r="F129" t="s">
+        <v>457</v>
+      </c>
+      <c r="G129">
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -4677,27 +4677,27 @@
         <v>270</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>67</v>
+        <v>131</v>
       </c>
       <c r="C131" t="s">
-        <v>19</v>
+        <v>465</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E131">
         <v>1</v>
       </c>
-      <c r="F131">
-        <v>0</v>
-      </c>
-      <c r="G131" t="s">
-        <v>457</v>
+      <c r="F131" t="s">
+        <v>457</v>
+      </c>
+      <c r="G131">
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -4729,14 +4729,14 @@
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>289</v>
+      <c r="A134" s="2" t="s">
+        <v>355</v>
       </c>
       <c r="B134" t="s">
-        <v>290</v>
+        <v>357</v>
       </c>
       <c r="C134" t="s">
-        <v>9</v>
+        <v>356</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>270</v>
@@ -4744,31 +4744,31 @@
       <c r="E134">
         <v>1</v>
       </c>
-      <c r="F134">
-        <v>0</v>
+      <c r="F134" t="s">
+        <v>457</v>
       </c>
       <c r="G134" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>284</v>
+      <c r="A135" s="2" t="s">
+        <v>473</v>
       </c>
       <c r="B135" t="s">
-        <v>285</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>286</v>
+        <v>474</v>
+      </c>
+      <c r="C135" t="s">
+        <v>466</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="E135">
         <v>1</v>
       </c>
-      <c r="F135">
-        <v>0</v>
+      <c r="F135" t="s">
+        <v>457</v>
       </c>
       <c r="G135" t="s">
         <v>457</v>
@@ -4789,14 +4789,14 @@
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
-        <v>294</v>
+      <c r="A137" t="s">
+        <v>377</v>
       </c>
       <c r="B137" t="s">
-        <v>295</v>
+        <v>378</v>
       </c>
       <c r="C137" t="s">
-        <v>296</v>
+        <v>207</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>270</v>
@@ -4804,31 +4804,31 @@
       <c r="E137">
         <v>1</v>
       </c>
-      <c r="F137">
-        <v>0</v>
+      <c r="F137" t="s">
+        <v>457</v>
       </c>
       <c r="G137" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="2" t="s">
-        <v>78</v>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>461</v>
       </c>
       <c r="B138" t="s">
-        <v>89</v>
+        <v>462</v>
       </c>
       <c r="C138" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="E138">
         <v>1</v>
       </c>
-      <c r="F138">
-        <v>0</v>
+      <c r="F138" t="s">
+        <v>457</v>
       </c>
       <c r="G138" t="s">
         <v>457</v>
@@ -4836,39 +4836,39 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>452</v>
+        <v>201</v>
       </c>
       <c r="B139" t="s">
-        <v>453</v>
+        <v>202</v>
       </c>
       <c r="C139" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>270</v>
+        <v>12</v>
       </c>
       <c r="E139">
         <v>1</v>
       </c>
-      <c r="F139">
-        <v>0</v>
-      </c>
-      <c r="G139" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="2" t="s">
-        <v>459</v>
+      <c r="F139" t="s">
+        <v>457</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>213</v>
       </c>
       <c r="B140" t="s">
-        <v>460</v>
+        <v>214</v>
       </c>
       <c r="C140" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E140">
         <v>1</v>
@@ -4876,31 +4876,31 @@
       <c r="F140">
         <v>0</v>
       </c>
-      <c r="G140" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>112</v>
+      <c r="G140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A141" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="B141" t="s">
-        <v>113</v>
+        <v>216</v>
       </c>
       <c r="C141" t="s">
-        <v>464</v>
+        <v>17</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E141">
         <v>1</v>
       </c>
-      <c r="F141" t="s">
-        <v>457</v>
-      </c>
-      <c r="G141" t="s">
-        <v>457</v>
+      <c r="F141">
+        <v>0</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -4945,50 +4945,50 @@
         <v>270</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="2" t="s">
-        <v>471</v>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>456</v>
       </c>
       <c r="B145" t="s">
-        <v>472</v>
+        <v>68</v>
       </c>
       <c r="C145" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E145">
         <v>1</v>
       </c>
-      <c r="F145" t="s">
-        <v>457</v>
-      </c>
-      <c r="G145" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>467</v>
+        <v>417</v>
       </c>
       <c r="B146" t="s">
-        <v>468</v>
+        <v>418</v>
       </c>
       <c r="C146" t="s">
-        <v>9</v>
+        <v>207</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>14</v>
+        <v>270</v>
       </c>
       <c r="E146">
         <v>1</v>
       </c>
-      <c r="F146" t="s">
-        <v>457</v>
-      </c>
-      <c r="G146" t="s">
-        <v>457</v>
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -5005,18 +5005,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>72</v>
+        <v>486</v>
       </c>
       <c r="B148" t="s">
-        <v>86</v>
+        <v>219</v>
       </c>
       <c r="C148" t="s">
-        <v>73</v>
+        <v>220</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="E148">
         <v>1</v>
@@ -5028,18 +5028,18 @@
         <v>457</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="2" t="s">
-        <v>475</v>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>15</v>
       </c>
       <c r="B149" t="s">
-        <v>476</v>
+        <v>16</v>
       </c>
       <c r="C149" t="s">
-        <v>465</v>
+        <v>17</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E149">
         <v>1</v>
@@ -5047,31 +5047,31 @@
       <c r="F149" t="s">
         <v>457</v>
       </c>
-      <c r="G149" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
-        <v>35</v>
+      <c r="G149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A150" s="2" t="s">
+        <v>343</v>
       </c>
       <c r="B150" t="s">
-        <v>36</v>
+        <v>344</v>
       </c>
       <c r="C150" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>13</v>
+        <v>270</v>
       </c>
       <c r="E150">
         <v>1</v>
       </c>
-      <c r="F150" t="s">
-        <v>457</v>
-      </c>
-      <c r="G150" t="s">
-        <v>457</v>
+      <c r="F150">
+        <v>0</v>
+      </c>
+      <c r="G150">
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -5102,64 +5102,64 @@
         <v>14</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>164</v>
+        <v>203</v>
       </c>
       <c r="B153" t="s">
-        <v>165</v>
+        <v>204</v>
       </c>
       <c r="C153" t="s">
-        <v>166</v>
+        <v>188</v>
       </c>
       <c r="D153" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+      <c r="F153" t="s">
+        <v>457</v>
+      </c>
+      <c r="G153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A154" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B154" t="s">
+        <v>155</v>
+      </c>
+      <c r="C154" t="s">
+        <v>9</v>
+      </c>
+      <c r="D154" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E153">
-        <v>1</v>
-      </c>
-      <c r="F153" t="s">
-        <v>457</v>
-      </c>
-      <c r="G153" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
-        <v>229</v>
-      </c>
-      <c r="B154" t="s">
-        <v>489</v>
-      </c>
-      <c r="C154" t="s">
-        <v>227</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E154">
         <v>1</v>
       </c>
       <c r="F154" t="s">
         <v>457</v>
       </c>
-      <c r="G154" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="2" t="s">
-        <v>76</v>
+      <c r="G154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>182</v>
       </c>
       <c r="B155" t="s">
-        <v>85</v>
+        <v>183</v>
       </c>
       <c r="C155" t="s">
-        <v>77</v>
+        <v>184</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="E155">
         <v>1</v>
@@ -5171,50 +5171,50 @@
         <v>457</v>
       </c>
     </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
-        <v>99</v>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A156" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="B156" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="C156" t="s">
-        <v>98</v>
+        <v>162</v>
       </c>
       <c r="D156" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156" t="s">
+        <v>457</v>
+      </c>
+      <c r="G156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>28</v>
+      </c>
+      <c r="B157" t="s">
+        <v>29</v>
+      </c>
+      <c r="C157" t="s">
+        <v>27</v>
+      </c>
+      <c r="D157" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E156">
-        <v>1</v>
-      </c>
-      <c r="F156" t="s">
-        <v>457</v>
-      </c>
-      <c r="G156" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
-        <v>193</v>
-      </c>
-      <c r="B157" t="s">
-        <v>194</v>
-      </c>
-      <c r="C157" t="s">
-        <v>188</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E157">
         <v>1</v>
       </c>
       <c r="F157" t="s">
         <v>457</v>
       </c>
-      <c r="G157" t="s">
-        <v>457</v>
+      <c r="G157">
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -5231,18 +5231,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
-        <v>46</v>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A159" s="2" t="s">
+        <v>303</v>
       </c>
       <c r="B159" t="s">
-        <v>47</v>
+        <v>304</v>
       </c>
       <c r="C159" t="s">
-        <v>21</v>
+        <v>305</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>18</v>
+        <v>270</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -5268,18 +5268,18 @@
         <v>270</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>232</v>
+        <v>446</v>
       </c>
       <c r="B161" t="s">
-        <v>233</v>
+        <v>447</v>
       </c>
       <c r="C161" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E161">
         <v>1</v>
@@ -5320,17 +5320,17 @@
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A164" s="2" t="s">
-        <v>297</v>
+      <c r="A164" t="s">
+        <v>105</v>
       </c>
       <c r="B164" t="s">
-        <v>298</v>
+        <v>106</v>
       </c>
       <c r="C164" t="s">
-        <v>299</v>
+        <v>464</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="E164">
         <v>1</v>
@@ -5342,27 +5342,27 @@
         <v>457</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="2" t="s">
-        <v>176</v>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>64</v>
       </c>
       <c r="B165" t="s">
-        <v>177</v>
+        <v>65</v>
       </c>
       <c r="C165" t="s">
-        <v>178</v>
+        <v>19</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E165">
         <v>1</v>
       </c>
-      <c r="F165" t="s">
-        <v>457</v>
-      </c>
-      <c r="G165" t="s">
-        <v>457</v>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="G165">
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -5379,15 +5379,15 @@
         <v>270</v>
       </c>
     </row>
-    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>211</v>
+        <v>258</v>
       </c>
       <c r="B167" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="C167" t="s">
-        <v>17</v>
+        <v>255</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>12</v>
@@ -5398,31 +5398,31 @@
       <c r="F167" t="s">
         <v>457</v>
       </c>
-      <c r="G167" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
-        <v>260</v>
+      <c r="G167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A168" s="2" t="s">
+        <v>324</v>
       </c>
       <c r="B168" t="s">
-        <v>261</v>
+        <v>325</v>
       </c>
       <c r="C168" t="s">
-        <v>255</v>
+        <v>326</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E168">
         <v>1</v>
       </c>
-      <c r="F168" t="s">
-        <v>457</v>
-      </c>
-      <c r="G168" t="s">
-        <v>457</v>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -5439,35 +5439,35 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>96</v>
+        <v>179</v>
       </c>
       <c r="B170" t="s">
-        <v>97</v>
+        <v>180</v>
       </c>
       <c r="C170" t="s">
-        <v>95</v>
+        <v>181</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E170">
         <v>1</v>
       </c>
-      <c r="F170" t="s">
-        <v>457</v>
-      </c>
-      <c r="G170" t="s">
-        <v>457</v>
+      <c r="F170">
+        <v>0</v>
+      </c>
+      <c r="G170">
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>401</v>
+        <v>452</v>
       </c>
       <c r="B171" t="s">
-        <v>402</v>
+        <v>453</v>
       </c>
       <c r="C171" t="s">
         <v>207</v>
@@ -5478,8 +5478,8 @@
       <c r="E171">
         <v>1</v>
       </c>
-      <c r="F171" t="s">
-        <v>457</v>
+      <c r="F171">
+        <v>0</v>
       </c>
       <c r="G171" t="s">
         <v>457</v>
@@ -5499,18 +5499,18 @@
         <v>270</v>
       </c>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="2" t="s">
-        <v>74</v>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>440</v>
       </c>
       <c r="B173" t="s">
-        <v>84</v>
+        <v>441</v>
       </c>
       <c r="C173" t="s">
-        <v>75</v>
+        <v>207</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>71</v>
+        <v>270</v>
       </c>
       <c r="E173">
         <v>1</v>
@@ -5518,22 +5518,22 @@
       <c r="F173" t="s">
         <v>457</v>
       </c>
-      <c r="G173" t="s">
-        <v>457</v>
+      <c r="G173">
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>275</v>
+        <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>277</v>
+        <v>174</v>
       </c>
       <c r="C174" t="s">
-        <v>276</v>
+        <v>175</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>270</v>
+        <v>14</v>
       </c>
       <c r="E174">
         <v>1</v>
@@ -5541,8 +5541,8 @@
       <c r="F174" t="s">
         <v>457</v>
       </c>
-      <c r="G174" t="s">
-        <v>457</v>
+      <c r="G174">
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -5559,15 +5559,15 @@
         <v>270</v>
       </c>
     </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>199</v>
+        <v>267</v>
       </c>
       <c r="B176" t="s">
-        <v>200</v>
+        <v>268</v>
       </c>
       <c r="C176" t="s">
-        <v>188</v>
+        <v>269</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>12</v>
@@ -5575,22 +5575,22 @@
       <c r="E176">
         <v>1</v>
       </c>
-      <c r="F176" t="s">
-        <v>457</v>
-      </c>
-      <c r="G176" t="s">
-        <v>457</v>
+      <c r="F176">
+        <v>0</v>
+      </c>
+      <c r="G176">
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A177" s="2" t="s">
-        <v>355</v>
+      <c r="A177" t="s">
+        <v>364</v>
       </c>
       <c r="B177" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="C177" t="s">
-        <v>356</v>
+        <v>207</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>270</v>
@@ -5601,19 +5601,19 @@
       <c r="F177" t="s">
         <v>457</v>
       </c>
-      <c r="G177" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="2" t="s">
-        <v>473</v>
+      <c r="G177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>170</v>
       </c>
       <c r="B178" t="s">
-        <v>474</v>
+        <v>171</v>
       </c>
       <c r="C178" t="s">
-        <v>466</v>
+        <v>172</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>14</v>
@@ -5624,16 +5624,16 @@
       <c r="F178" t="s">
         <v>457</v>
       </c>
-      <c r="G178" t="s">
-        <v>457</v>
+      <c r="G178">
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>377</v>
+        <v>411</v>
       </c>
       <c r="B179" t="s">
-        <v>378</v>
+        <v>412</v>
       </c>
       <c r="C179" t="s">
         <v>207</v>
@@ -5647,8 +5647,8 @@
       <c r="F179" t="s">
         <v>457</v>
       </c>
-      <c r="G179" t="s">
-        <v>457</v>
+      <c r="G179">
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -5693,41 +5693,41 @@
         <v>270</v>
       </c>
     </row>
-    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>461</v>
+        <v>429</v>
       </c>
       <c r="B183" t="s">
-        <v>462</v>
+        <v>490</v>
       </c>
       <c r="C183" t="s">
-        <v>45</v>
+        <v>207</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>13</v>
+        <v>270</v>
       </c>
       <c r="E183">
         <v>1</v>
       </c>
-      <c r="F183" t="s">
-        <v>457</v>
-      </c>
-      <c r="G183" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F183">
+        <v>1</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>486</v>
+        <v>88</v>
       </c>
       <c r="B184" t="s">
-        <v>219</v>
+        <v>87</v>
       </c>
       <c r="C184" t="s">
-        <v>220</v>
+        <v>70</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -5735,19 +5735,19 @@
       <c r="F184" t="s">
         <v>457</v>
       </c>
-      <c r="G184" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="G184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="B185" t="s">
-        <v>183</v>
+        <v>104</v>
       </c>
       <c r="C185" t="s">
-        <v>184</v>
+        <v>464</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>14</v>
@@ -5777,14 +5777,14 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A187" s="2" t="s">
-        <v>303</v>
+      <c r="A187" t="s">
+        <v>423</v>
       </c>
       <c r="B187" t="s">
-        <v>304</v>
+        <v>424</v>
       </c>
       <c r="C187" t="s">
-        <v>305</v>
+        <v>207</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>270</v>
@@ -5792,11 +5792,11 @@
       <c r="E187">
         <v>1</v>
       </c>
-      <c r="F187" t="s">
-        <v>457</v>
-      </c>
-      <c r="G187" t="s">
-        <v>457</v>
+      <c r="F187">
+        <v>0</v>
+      </c>
+      <c r="G187">
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
@@ -5829,16 +5829,16 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>446</v>
+        <v>251</v>
       </c>
       <c r="B190" t="s">
-        <v>447</v>
+        <v>252</v>
       </c>
       <c r="C190" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>270</v>
+        <v>12</v>
       </c>
       <c r="E190">
         <v>1</v>
@@ -5850,18 +5850,18 @@
         <v>457</v>
       </c>
     </row>
-    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>105</v>
+        <v>249</v>
       </c>
       <c r="B191" t="s">
-        <v>106</v>
+        <v>250</v>
       </c>
       <c r="C191" t="s">
-        <v>464</v>
+        <v>227</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E191">
         <v>1</v>
@@ -5873,18 +5873,18 @@
         <v>457</v>
       </c>
     </row>
-    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>103</v>
+        <v>208</v>
       </c>
       <c r="B192" t="s">
-        <v>104</v>
+        <v>209</v>
       </c>
       <c r="C192" t="s">
-        <v>464</v>
+        <v>210</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E192">
         <v>1</v>
@@ -5938,18 +5938,18 @@
         <v>270</v>
       </c>
     </row>
-    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
-        <v>251</v>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A196" s="2" t="s">
+        <v>313</v>
       </c>
       <c r="B196" t="s">
-        <v>252</v>
+        <v>314</v>
       </c>
       <c r="C196" t="s">
-        <v>227</v>
+        <v>315</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>12</v>
+        <v>270</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -5961,12 +5961,12 @@
         <v>457</v>
       </c>
     </row>
-    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B197" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C197" t="s">
         <v>227</v>
@@ -5984,18 +5984,18 @@
         <v>457</v>
       </c>
     </row>
-    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>208</v>
+        <v>483</v>
       </c>
       <c r="B198" t="s">
-        <v>209</v>
+        <v>484</v>
       </c>
       <c r="C198" t="s">
-        <v>210</v>
+        <v>465</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E198">
         <v>1</v>
@@ -6003,22 +6003,22 @@
       <c r="F198" t="s">
         <v>457</v>
       </c>
-      <c r="G198" t="s">
-        <v>457</v>
+      <c r="G198">
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A199" s="2" t="s">
-        <v>313</v>
+      <c r="A199" t="s">
+        <v>41</v>
       </c>
       <c r="B199" t="s">
-        <v>314</v>
+        <v>42</v>
       </c>
       <c r="C199" t="s">
-        <v>315</v>
+        <v>40</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>270</v>
+        <v>13</v>
       </c>
       <c r="E199">
         <v>1</v>
@@ -6030,18 +6030,18 @@
         <v>457</v>
       </c>
     </row>
-    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>253</v>
-      </c>
-      <c r="B200" t="s">
-        <v>254</v>
+        <v>23</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C200" t="s">
-        <v>227</v>
+        <v>9</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E200">
         <v>1</v>
@@ -6053,15 +6053,15 @@
         <v>457</v>
       </c>
     </row>
-    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A201" t="s">
-        <v>41</v>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A201" s="2" t="s">
+        <v>459</v>
       </c>
       <c r="B201" t="s">
-        <v>42</v>
+        <v>460</v>
       </c>
       <c r="C201" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>13</v>
@@ -6069,50 +6069,45 @@
       <c r="E201">
         <v>1</v>
       </c>
-      <c r="F201" t="s">
-        <v>457</v>
+      <c r="F201">
+        <v>0</v>
       </c>
       <c r="G201" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>23</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>25</v>
+        <v>146</v>
+      </c>
+      <c r="B202" t="s">
+        <v>147</v>
       </c>
       <c r="C202" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E202">
         <v>1</v>
       </c>
-      <c r="F202" t="s">
-        <v>457</v>
-      </c>
-      <c r="G202" t="s">
-        <v>457</v>
+      <c r="F202">
+        <v>0</v>
+      </c>
+      <c r="G202">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G202" xr:uid="{AA8F527B-D131-4489-90F2-792A2C6B7552}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Papunesia"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="4">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
     <sortState ref="A2:G202">
-      <sortCondition ref="G1:G202"/>
+      <sortCondition ref="A1:A202"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>